<commit_message>
Added basic files for project as well as element list in excel sheet
</commit_message>
<xml_diff>
--- a/featureList.xlsx
+++ b/featureList.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanholmes/Documents/HREXT Projects/hrext04-my-cruddy-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37E3F8CE-50AD-B344-8AF1-1BA7F2455DAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1703C688-91FC-4546-82D8-256A961DD66F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16100" xr2:uid="{375A94D2-1DA6-794E-88E4-AA31F2A60890}"/>
+    <workbookView xWindow="0" yWindow="8520" windowWidth="28800" windowHeight="8060" xr2:uid="{375A94D2-1DA6-794E-88E4-AA31F2A60890}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>input field for text to memorize</t>
   </si>
@@ -93,6 +93,93 @@
   </si>
   <si>
     <t>edit voice-to-text output</t>
+  </si>
+  <si>
+    <t>FONT END ELEMENT</t>
+  </si>
+  <si>
+    <t>BACK END DEPENDENCIES</t>
+  </si>
+  <si>
+    <t>Source Text input field</t>
+  </si>
+  <si>
+    <t>ELEMENT TAG</t>
+  </si>
+  <si>
+    <t>textArea</t>
+  </si>
+  <si>
+    <t>DATATYPE</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>Object normal/stripped and chunked</t>
+  </si>
+  <si>
+    <t>Start Button</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>Start/Stop Record Btn</t>
+  </si>
+  <si>
+    <t>currentVoiceText</t>
+  </si>
+  <si>
+    <t>Web Speach API</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>?? div/input?</t>
+  </si>
+  <si>
+    <t>Voice Text Display (editabe)</t>
+  </si>
+  <si>
+    <t>Compare button</t>
+  </si>
+  <si>
+    <t>currentChunkIndex</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Display comparison</t>
+  </si>
+  <si>
+    <t>missedWords</t>
+  </si>
+  <si>
+    <t>array[string]</t>
+  </si>
+  <si>
+    <t>extraWords</t>
+  </si>
+  <si>
+    <t>Display correct chunk</t>
+  </si>
+  <si>
+    <t>chunks</t>
+  </si>
+  <si>
+    <t>sourceText</t>
+  </si>
+  <si>
+    <t>Reset button</t>
+  </si>
+  <si>
+    <t>Next button</t>
+  </si>
+  <si>
+    <t>Previous button</t>
   </si>
 </sst>
 </file>
@@ -124,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -132,13 +219,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,18 +551,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A977EB-A962-F24B-B141-D7B1255D100E}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -474,8 +576,20 @@
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,8 +599,14 @@
       <c r="C2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -496,28 +616,76 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -527,8 +695,17 @@
       <c r="C8">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -538,8 +715,14 @@
       <c r="C9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -549,8 +732,14 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -560,8 +749,17 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -571,8 +769,14 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -582,8 +786,17 @@
       <c r="C13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -593,8 +806,14 @@
       <c r="C14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -604,8 +823,17 @@
       <c r="C15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -615,8 +843,17 @@
       <c r="C16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -626,8 +863,14 @@
       <c r="C17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -637,8 +880,25 @@
       <c r="C18">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>